<commit_message>
add second sheet in excel file
</commit_message>
<xml_diff>
--- a/backend/src/media/investment_projects.xlsx
+++ b/backend/src/media/investment_projects.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Инвестиционные_проекты" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Статистика" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,6 +426,81 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Название проекта</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Кол-во создаваемых рабочих мест</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Общая стоимость инвестиционного проекта, млн. руб</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>HUI</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Ta ya togo se</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Mafioznik</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>26</v>
+      </c>
+      <c r="C4" t="n">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -436,44 +512,44 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Название проекта</t>
+          <t>Отрасль</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Кол-во создаваемых рабочих мест</t>
+          <t>Кол-во проектов</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Общая стоимость инвестиционного проекта, млн. руб</t>
+          <t>Сумма инвестиций по отрасли</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HUI</t>
+          <t>станкоинструментальная промышленность</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>hui2</t>
+          <t>сельскохозяйственное машиностроение</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>